<commit_message>
Update Config and Fix Outlook_SendEmail
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Panda\Documents\UiPath\Final Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npanda5\Documents\UiPath\Activity\Final Project\Final Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94D117C-6908-44FC-BD07-532DDD6C0A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E9019E-D64E-49E6-96AE-CD297A3B2BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-2895" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -178,13 +178,19 @@
   </si>
   <si>
     <t>https://www.amazon.com/</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>naim.panda@dxc.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -208,12 +214,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,9 +232,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -246,10 +245,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,7 +563,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -667,7 +665,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1652,11 +1657,8 @@
     <row r="993" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{D8D38056-1557-4C0A-9C24-4A02389B2B58}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fix Outlook and add other Amazon component folders
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npanda5\Documents\UiPath\Activity\Final Project\Final Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npanda5\Documents\UiPath\Activity\Final Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E9019E-D64E-49E6-96AE-CD297A3B2BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD49AF36-3B8B-4B51-983F-C498339BB221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
     <t>Recipient</t>
   </si>
   <si>
-    <t>naim.panda@dxc.com</t>
+    <t>naim.panda@dxc.com; karlvincent.maranan@dxc.com</t>
   </si>
 </sst>
 </file>
@@ -563,13 +563,13 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Fix Header - Format Cell
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npanda5\Documents\UiPath\Activity\Final Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Panda\Documents\UiPath\Final Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0682F243-E366-4C20-BB01-C5B3E68B9E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEE7F8C-731A-4668-949A-6A62E0E89537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-2895" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Add Cc on Outlook
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Panda\Documents\UiPath\Final Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npanda5\Documents\UiPath\Activity\Final Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8E95DB-08BF-46E3-B585-7A1BD98E0BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D746C8A-8A0C-4502-A2E1-B439F0EFF870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-2895" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>naim.panda@dxc.com</t>
+  </si>
+  <si>
+    <t>Cc</t>
+  </si>
+  <si>
+    <t>karlvincent.maranan@dxc.com</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -673,7 +679,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>